<commit_message>
Added more CSV files
</commit_message>
<xml_diff>
--- a/Excel Documents/Afgelegde ritten per chauffeur.xlsx
+++ b/Excel Documents/Afgelegde ritten per chauffeur.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelkolb/Library/Containers/com.apple.mail/Data/Library/Mail Downloads/AA7AD075-932B-4171-88A9-AFE4E1629004/Excel Samuel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelkolb/Documents/PhD/Excel/Excel Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23480" windowHeight="15700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Open" sheetId="1" r:id="rId1"/>
     <sheet name="Solved" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="16">
   <si>
     <t>Chauffeur</t>
   </si>
@@ -71,12 +74,15 @@
   <si>
     <t>?</t>
   </si>
+  <si>
+    <t>Chauffeur:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +102,13 @@
       <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -119,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -127,6 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,24 +473,12 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -484,6 +486,9 @@
       </c>
       <c r="B4" s="1">
         <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
@@ -1207,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1233,24 +1238,12 @@
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1259,6 +1252,9 @@
       <c r="B4" s="1">
         <v>16</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1289,27 +1285,27 @@
         <v>9</v>
       </c>
       <c r="E5" s="4">
-        <f>SUMIF($A$4:$A$77,E4,$B$4:$B$77)</f>
+        <f t="shared" ref="E5:J5" si="0">SUMIF($A$4:$A$77,E4,$B$4:$B$77)</f>
         <v>1027</v>
       </c>
       <c r="F5" s="4">
-        <f>SUMIF($A$4:$A$77,F4,$B$4:$B$77)</f>
+        <f t="shared" si="0"/>
         <v>712</v>
       </c>
       <c r="G5" s="4">
-        <f>SUMIF($A$4:$A$77,G4,$B$4:$B$77)</f>
+        <f t="shared" si="0"/>
         <v>630</v>
       </c>
       <c r="H5" s="4">
-        <f>SUMIF($A$4:$A$77,H4,$B$4:$B$77)</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="I5" s="4">
-        <f>SUMIF($A$4:$A$77,I4,$B$4:$B$77)</f>
+        <f t="shared" si="0"/>
         <v>797</v>
       </c>
       <c r="J5" s="4">
-        <f>SUMIF($A$4:$A$77,J4,$B$4:$B$77)</f>
+        <f t="shared" si="0"/>
         <v>586</v>
       </c>
     </row>
@@ -1328,23 +1324,23 @@
         <v>54.05263157894737</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6:J6" si="0">AVERAGEIF($A$4:$A$77,F4,$B$4:$B$77)</f>
+        <f t="shared" ref="F6:J6" si="1">AVERAGEIF($A$4:$A$77,F4,$B$4:$B$77)</f>
         <v>64.727272727272734</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66.416666666666671</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48.833333333333336</v>
       </c>
     </row>
@@ -1359,27 +1355,27 @@
         <v>11</v>
       </c>
       <c r="E7" s="4">
-        <f>COUNTIF($A$4:$A$77, E4)</f>
+        <f t="shared" ref="E7:J7" si="2">COUNTIF($A$4:$A$77, E4)</f>
         <v>19</v>
       </c>
       <c r="F7" s="4">
-        <f>COUNTIF($A$4:$A$77, F4)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G7" s="4">
-        <f>COUNTIF($A$4:$A$77, G4)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="H7" s="4">
-        <f>COUNTIF($A$4:$A$77, H4)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="I7" s="4">
-        <f>COUNTIF($A$4:$A$77, I4)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J7" s="4">
-        <f>COUNTIF($A$4:$A$77, J4)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
     </row>

</xml_diff>